<commit_message>
Finished version of smallGR
</commit_message>
<xml_diff>
--- a/projects/CGE_Generator/data/IO2018/GR2018_mappings.xlsx
+++ b/projects/CGE_Generator/data/IO2018/GR2018_mappings.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxj477\Documents\GitHub\GPM_v07\projects\CGE_Generator\data\IO2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxj477\Documents\GitHub\GPM_v071\projects\CGE_Generator\data\IO2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Energivaremapping" sheetId="1" r:id="rId1"/>
     <sheet name="AuxMaps" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="245">
   <si>
     <t>LVN</t>
   </si>
@@ -730,13 +731,47 @@
   </si>
   <si>
     <t>iM</t>
+  </si>
+  <si>
+    <t>GreenREFORM</t>
+  </si>
+  <si>
+    <t>IO total value</t>
+  </si>
+  <si>
+    <t>IO buildings</t>
+  </si>
+  <si>
+    <t>s146, 1000DKK</t>
+  </si>
+  <si>
+    <t>19000, GreenREFORM:</t>
+  </si>
+  <si>
+    <t>qK</t>
+  </si>
+  <si>
+    <t>pK</t>
+  </si>
+  <si>
+    <t>vK</t>
+  </si>
+  <si>
+    <t>vY</t>
+  </si>
+  <si>
+    <t>19000, IO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -764,16 +799,36 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -781,12 +836,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -794,8 +861,12 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -1077,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2543,8 +2614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4667,4 +4738,264 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A9:XFD43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>239</v>
+      </c>
+      <c r="G9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>240</v>
+      </c>
+      <c r="D10">
+        <v>4.4169047206419201</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>241</v>
+      </c>
+      <c r="D11">
+        <v>0.152467188683547</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D12">
+        <f>D11*D10</f>
+        <v>0.67343304543936111</v>
+      </c>
+      <c r="G12">
+        <v>4.3380000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>243</v>
+      </c>
+      <c r="D13">
+        <v>34.336990240680102</v>
+      </c>
+      <c r="G13" s="6">
+        <v>34.338533566780789</v>
+      </c>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>238</v>
+      </c>
+      <c r="B22" t="s">
+        <v>236</v>
+      </c>
+      <c r="C22" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>190000</v>
+      </c>
+      <c r="B23" s="5">
+        <v>34338533.566780791</v>
+      </c>
+      <c r="C23" s="6">
+        <v>4338000</v>
+      </c>
+      <c r="E23">
+        <f>C23/B23</f>
+        <v>0.12633038017082346</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>210000</v>
+      </c>
+      <c r="B24" s="6">
+        <v>123818164.36256719</v>
+      </c>
+      <c r="C24" s="6">
+        <v>35883000</v>
+      </c>
+      <c r="E24">
+        <f>C24/B24</f>
+        <v>0.28980400561363984</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>236</v>
+      </c>
+      <c r="C26" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>10929820.001952305</v>
+      </c>
+      <c r="C27">
+        <v>103681000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>12285048.003851051</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>2795438.0268147779</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>3557806.7200454632</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>6195053.0013932055</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>199900.00016106479</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <f>SUM(B27:B32)/1000000</f>
+        <v>35.963065754217865</v>
+      </c>
+      <c r="C34">
+        <f>SUM(C27:C32)/1000000</f>
+        <v>103.681</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>10.929820000976701</v>
+      </c>
+      <c r="C36">
+        <v>32.759602675278302</v>
+      </c>
+      <c r="E36">
+        <v>0.14714791400463401</v>
+      </c>
+      <c r="F36">
+        <f>SUMPRODUCT(C36:C41,E36:E41)</f>
+        <v>13.184459099797163</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>12.2850480050696</v>
+      </c>
+      <c r="C37">
+        <v>37.113965721083602</v>
+      </c>
+      <c r="E37">
+        <v>0.116052015551017</v>
+      </c>
+      <c r="XFD37" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>2.7954380271300101</v>
+      </c>
+      <c r="C38">
+        <v>8.4046219108920006</v>
+      </c>
+      <c r="E38">
+        <v>0.112781099136364</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>3.5565266203839001</v>
+      </c>
+      <c r="C39">
+        <v>11.45736981436</v>
+      </c>
+      <c r="E39">
+        <v>0.115812478313835</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>6.1950530016887804</v>
+      </c>
+      <c r="C40">
+        <v>16.9462654869909</v>
+      </c>
+      <c r="E40">
+        <v>0.101746009573734</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>0.19990000035487701</v>
+      </c>
+      <c r="C41">
+        <v>0.50659134056553001</v>
+      </c>
+      <c r="E41">
+        <v>0.11409116241143601</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <f>SUM(B36:B41)</f>
+        <v>35.961785655603869</v>
+      </c>
+      <c r="C43">
+        <f>SUM(C36:C41)</f>
+        <v>107.18841694917033</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>